<commit_message>
feat: added status e-mails
</commit_message>
<xml_diff>
--- a/PipelineWorksheet.xlsx
+++ b/PipelineWorksheet.xlsx
@@ -27,15 +27,9 @@
     <t>Run_Name</t>
   </si>
   <si>
-    <t>230711_N_I_063</t>
-  </si>
-  <si>
     <t>Run_Dir</t>
   </si>
   <si>
-    <t>/nfs/APL_Genomics/230711_N_I_063/</t>
-  </si>
-  <si>
     <t>Seq_Type</t>
   </si>
   <si>
@@ -451,6 +445,12 @@
   </si>
   <si>
     <t>/nfs/Genomics_DEV/projects/alindsay/Projects/seq-sample-split/results/ww</t>
+  </si>
+  <si>
+    <t>230713_N_I_064</t>
+  </si>
+  <si>
+    <t>/nfs/Genomics_DEV/projects/alindsay/Projects/seq-sample-split/data/</t>
   </si>
 </sst>
 </file>
@@ -1647,8 +1647,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1667,278 +1667,278 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>142</v>
       </c>
       <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>4</v>
+        <v>143</v>
       </c>
       <c r="D3" s="27"/>
     </row>
     <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>5</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="27" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="28" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D7" s="29"/>
     </row>
     <row r="8" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D8" s="30"/>
     </row>
     <row r="9" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D9" s="31"/>
     </row>
     <row r="10" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="31"/>
     </row>
     <row r="11" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="31"/>
     </row>
     <row r="12" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="31"/>
     </row>
     <row r="13" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" s="31"/>
     </row>
     <row r="14" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D14" s="31"/>
     </row>
     <row r="15" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="31"/>
     </row>
     <row r="19" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D19" s="32"/>
     </row>
     <row r="21" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D21" s="33"/>
     </row>
     <row r="22" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D22" s="34"/>
     </row>
     <row r="23" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D23" s="35"/>
     </row>
     <row r="24" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D24" s="35"/>
     </row>
     <row r="25" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D25" s="35"/>
     </row>
     <row r="26" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D26" s="35"/>
     </row>
     <row r="27" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D27" s="35"/>
     </row>
     <row r="28" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D28" s="35"/>
     </row>
     <row r="29" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D29" s="35"/>
     </row>
     <row r="30" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D30" s="35"/>
     </row>
     <row r="31" spans="1:4" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D31" s="35"/>
     </row>
     <row r="32" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D32" s="36"/>
     </row>
     <row r="34" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D34" s="37"/>
     </row>
     <row r="35" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B35" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" s="24" t="s">
         <v>16</v>
-      </c>
-      <c r="B35" s="24" t="s">
-        <v>140</v>
-      </c>
-      <c r="C35" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.25">
@@ -1946,10 +1946,10 @@
         <v>1</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -1957,10 +1957,10 @@
         <v>2</v>
       </c>
       <c r="B37" s="43" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C37" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -1968,7 +1968,7 @@
         <v>3</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -1976,7 +1976,7 @@
         <v>4</v>
       </c>
       <c r="B39" s="43" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -1984,7 +1984,7 @@
         <v>5</v>
       </c>
       <c r="B40" s="43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -1992,7 +1992,7 @@
         <v>6</v>
       </c>
       <c r="B41" s="43" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2000,13 +2000,13 @@
         <v>7</v>
       </c>
       <c r="B42" s="43" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C42" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D42" s="44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2014,13 +2014,13 @@
         <v>8</v>
       </c>
       <c r="B43" s="43" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C43" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D43" s="44" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2028,13 +2028,13 @@
         <v>9</v>
       </c>
       <c r="B44" s="43" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D44" s="44" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2042,10 +2042,10 @@
         <v>10</v>
       </c>
       <c r="B45" s="43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D45" s="44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2053,10 +2053,10 @@
         <v>11</v>
       </c>
       <c r="B46" s="43" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C46" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2064,10 +2064,10 @@
         <v>12</v>
       </c>
       <c r="B47" s="43" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C47" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2075,7 +2075,7 @@
         <v>13</v>
       </c>
       <c r="B48" s="43" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="49" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2083,7 +2083,7 @@
         <v>14</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2091,7 +2091,7 @@
         <v>15</v>
       </c>
       <c r="B50" s="43" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2099,7 +2099,7 @@
         <v>16</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2107,7 +2107,7 @@
         <v>17</v>
       </c>
       <c r="B52" s="43" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2115,7 +2115,7 @@
         <v>18</v>
       </c>
       <c r="B53" s="43" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="54" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2123,7 +2123,7 @@
         <v>19</v>
       </c>
       <c r="B54" s="43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="55" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2131,7 +2131,7 @@
         <v>20</v>
       </c>
       <c r="B55" s="43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2139,7 +2139,7 @@
         <v>21</v>
       </c>
       <c r="B56" s="43" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="57" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2147,7 +2147,7 @@
         <v>22</v>
       </c>
       <c r="B57" s="43" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2155,7 +2155,7 @@
         <v>23</v>
       </c>
       <c r="B58" s="43" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2163,7 +2163,7 @@
         <v>24</v>
       </c>
       <c r="B59" s="43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
         <v>25</v>
       </c>
       <c r="B60" s="43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
         <v>26</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2187,7 +2187,7 @@
         <v>27</v>
       </c>
       <c r="B62" s="43" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2195,7 +2195,7 @@
         <v>28</v>
       </c>
       <c r="B63" s="43" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2203,7 +2203,7 @@
         <v>29</v>
       </c>
       <c r="B64" s="43" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2211,7 +2211,7 @@
         <v>30</v>
       </c>
       <c r="B65" s="43" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="66" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2219,13 +2219,13 @@
         <v>31</v>
       </c>
       <c r="B66" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C66" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D66" s="44" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="67" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2233,13 +2233,13 @@
         <v>32</v>
       </c>
       <c r="B67" s="43" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C67" s="44" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D67" s="44" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2247,7 +2247,7 @@
         <v>33</v>
       </c>
       <c r="B68" s="43" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2255,7 +2255,7 @@
         <v>34</v>
       </c>
       <c r="B69" s="43" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="70" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2263,7 +2263,7 @@
         <v>35</v>
       </c>
       <c r="B70" s="43" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2271,7 +2271,7 @@
         <v>36</v>
       </c>
       <c r="B71" s="43" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2279,7 +2279,7 @@
         <v>37</v>
       </c>
       <c r="B72" s="43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2287,7 +2287,7 @@
         <v>38</v>
       </c>
       <c r="B73" s="43" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="74" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2295,7 +2295,7 @@
         <v>39</v>
       </c>
       <c r="B74" s="43" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2303,7 +2303,7 @@
         <v>40</v>
       </c>
       <c r="B75" s="43" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2311,7 +2311,7 @@
         <v>41</v>
       </c>
       <c r="B76" s="43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2319,7 +2319,7 @@
         <v>42</v>
       </c>
       <c r="B77" s="43" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2327,7 +2327,7 @@
         <v>43</v>
       </c>
       <c r="B78" s="43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2335,7 +2335,7 @@
         <v>44</v>
       </c>
       <c r="B79" s="43" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:4" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2343,7 +2343,7 @@
         <v>45</v>
       </c>
       <c r="B80" s="43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2351,7 +2351,7 @@
         <v>46</v>
       </c>
       <c r="B81" s="43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
         <v>47</v>
       </c>
       <c r="B82" s="43" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2367,7 +2367,7 @@
         <v>48</v>
       </c>
       <c r="B83" s="43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2375,7 +2375,7 @@
         <v>49</v>
       </c>
       <c r="B84" s="43" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2383,7 +2383,7 @@
         <v>50</v>
       </c>
       <c r="B85" s="43" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2391,7 +2391,7 @@
         <v>51</v>
       </c>
       <c r="B86" s="43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2399,7 +2399,7 @@
         <v>52</v>
       </c>
       <c r="B87" s="43" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2407,7 +2407,7 @@
         <v>53</v>
       </c>
       <c r="B88" s="43" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2415,7 +2415,7 @@
         <v>54</v>
       </c>
       <c r="B89" s="43" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2423,7 +2423,7 @@
         <v>55</v>
       </c>
       <c r="B90" s="43" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2431,7 +2431,7 @@
         <v>56</v>
       </c>
       <c r="B91" s="43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2439,7 +2439,7 @@
         <v>57</v>
       </c>
       <c r="B92" s="43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2447,7 +2447,7 @@
         <v>58</v>
       </c>
       <c r="B93" s="43" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2455,7 +2455,7 @@
         <v>59</v>
       </c>
       <c r="B94" s="43" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2463,7 +2463,7 @@
         <v>60</v>
       </c>
       <c r="B95" s="43" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2471,7 +2471,7 @@
         <v>61</v>
       </c>
       <c r="B96" s="43" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2479,7 +2479,7 @@
         <v>62</v>
       </c>
       <c r="B97" s="43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
         <v>63</v>
       </c>
       <c r="B98" s="43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>64</v>
       </c>
       <c r="B99" s="43" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
         <v>65</v>
       </c>
       <c r="B100" s="43" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="101" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2511,7 +2511,7 @@
         <v>66</v>
       </c>
       <c r="B101" s="43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2519,7 +2519,7 @@
         <v>67</v>
       </c>
       <c r="B102" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2527,7 +2527,7 @@
         <v>68</v>
       </c>
       <c r="B103" s="43" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2535,7 +2535,7 @@
         <v>69</v>
       </c>
       <c r="B104" s="43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2543,7 +2543,7 @@
         <v>70</v>
       </c>
       <c r="B105" s="43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="106" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2551,7 +2551,7 @@
         <v>71</v>
       </c>
       <c r="B106" s="43" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="107" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2559,7 +2559,7 @@
         <v>72</v>
       </c>
       <c r="B107" s="43" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="108" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2567,7 +2567,7 @@
         <v>73</v>
       </c>
       <c r="B108" s="43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="109" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2575,7 +2575,7 @@
         <v>74</v>
       </c>
       <c r="B109" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="110" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2583,7 +2583,7 @@
         <v>75</v>
       </c>
       <c r="B110" s="43" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="111" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2591,7 +2591,7 @@
         <v>76</v>
       </c>
       <c r="B111" s="43" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="112" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2599,7 +2599,7 @@
         <v>77</v>
       </c>
       <c r="B112" s="43" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="113" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2607,7 +2607,7 @@
         <v>78</v>
       </c>
       <c r="B113" s="43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="114" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2615,7 +2615,7 @@
         <v>79</v>
       </c>
       <c r="B114" s="43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="115" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2623,7 +2623,7 @@
         <v>80</v>
       </c>
       <c r="B115" s="43" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="116" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2631,7 +2631,7 @@
         <v>81</v>
       </c>
       <c r="B116" s="43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="117" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2639,7 +2639,7 @@
         <v>82</v>
       </c>
       <c r="B117" s="43" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="118" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
         <v>83</v>
       </c>
       <c r="B118" s="43" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="119" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2655,7 +2655,7 @@
         <v>84</v>
       </c>
       <c r="B119" s="43" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2663,7 +2663,7 @@
         <v>85</v>
       </c>
       <c r="B120" s="43" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>86</v>
       </c>
       <c r="B121" s="43" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="122" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2679,7 +2679,7 @@
         <v>87</v>
       </c>
       <c r="B122" s="43" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="123" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
         <v>88</v>
       </c>
       <c r="B123" s="43" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="124" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2695,7 +2695,7 @@
         <v>89</v>
       </c>
       <c r="B124" s="43" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="125" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2703,7 +2703,7 @@
         <v>90</v>
       </c>
       <c r="B125" s="43" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="126" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2711,7 +2711,7 @@
         <v>91</v>
       </c>
       <c r="B126" s="43" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="127" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
         <v>92</v>
       </c>
       <c r="B127" s="43" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="128" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2727,7 +2727,7 @@
         <v>93</v>
       </c>
       <c r="B128" s="43" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="129" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2735,7 +2735,7 @@
         <v>94</v>
       </c>
       <c r="B129" s="43" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="130" spans="1:7" s="44" customFormat="1" x14ac:dyDescent="0.25">
@@ -2743,7 +2743,7 @@
         <v>95</v>
       </c>
       <c r="B130" s="43" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="131" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>96</v>
       </c>
       <c r="B131" s="46" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>